<commit_message>
Crated a normalized sheet for geo analysis
</commit_message>
<xml_diff>
--- a/viz/Beijing_AirQuality_Stations_en.xlsx
+++ b/viz/Beijing_AirQuality_Stations_en.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\数据竞赛\KDD Cup 2018\historical data\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leosa_000\Documents\GitHub\DS420-Cobras\viz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51FF6211-16A7-44E9-80E7-164760F946F7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{456021F0-1A90-403C-A04E-E00C3E5283DB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Normalized" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
   <si>
     <t>type</t>
   </si>
@@ -246,30 +246,45 @@
     <t>Urban Stations</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Urban</t>
+  </si>
+  <si>
+    <t>StationType</t>
+  </si>
+  <si>
+    <t>Suburban</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Traffic</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -356,7 +371,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -373,30 +388,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -412,7 +430,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -707,30 +725,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491A045D-4A9D-4511-A6A7-F29AC10F5C98}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.46484375" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="13.86328125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" ht="53.25" customHeight="1" thickBot="1">
+      <c r="A1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -738,72 +756,72 @@
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:4" ht="45" customHeight="1" thickBot="1">
+      <c r="A10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
@@ -814,15 +832,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:4" ht="18" thickBot="1">
+      <c r="A12" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.65" thickBot="1">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
@@ -833,7 +851,7 @@
         <v>39.929000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.65" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -844,7 +862,7 @@
         <v>39.886000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="14.65" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -855,7 +873,7 @@
         <v>39.929000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.65" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -866,7 +884,7 @@
         <v>39.878</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="14.65" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -877,7 +895,7 @@
         <v>39.981999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="14.65" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -888,7 +906,7 @@
         <v>39.936999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="14.65" thickBot="1">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
@@ -899,7 +917,7 @@
         <v>39.987000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="14.65" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
@@ -910,7 +928,7 @@
         <v>40.090000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="14.65" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
@@ -921,7 +939,7 @@
         <v>40.002000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="14.65" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -932,7 +950,7 @@
         <v>39.863</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="14.65" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -943,7 +961,7 @@
         <v>39.823999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
@@ -954,20 +972,20 @@
         <v>39.914000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" ht="18" thickBot="1">
+      <c r="A26" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="14.65" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>19</v>
       </c>
@@ -978,7 +996,7 @@
         <v>39.741999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="14.65" thickBot="1">
       <c r="A28" s="5" t="s">
         <v>20</v>
       </c>
@@ -989,7 +1007,7 @@
         <v>39.718000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="14.65" thickBot="1">
       <c r="A29" s="5" t="s">
         <v>21</v>
       </c>
@@ -1000,7 +1018,7 @@
         <v>39.795000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="14.65" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>22</v>
       </c>
@@ -1011,7 +1029,7 @@
         <v>39.886000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="14.65" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>23</v>
       </c>
@@ -1022,7 +1040,7 @@
         <v>40.127000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="14.65" thickBot="1">
       <c r="A32" s="5" t="s">
         <v>24</v>
       </c>
@@ -1033,7 +1051,7 @@
         <v>40.216999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="14.65" thickBot="1">
       <c r="A33" s="5" t="s">
         <v>25</v>
       </c>
@@ -1044,7 +1062,7 @@
         <v>39.936999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="14.65" thickBot="1">
       <c r="A34" s="5" t="s">
         <v>26</v>
       </c>
@@ -1055,7 +1073,7 @@
         <v>40.143000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="14.65" thickBot="1">
       <c r="A35" s="5" t="s">
         <v>27</v>
       </c>
@@ -1066,7 +1084,7 @@
         <v>40.328000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="14.65" thickBot="1">
       <c r="A36" s="5" t="s">
         <v>28</v>
       </c>
@@ -1077,7 +1095,7 @@
         <v>40.369999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="5" t="s">
         <v>29</v>
       </c>
@@ -1088,20 +1106,20 @@
         <v>40.453000000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" ht="18" thickBot="1">
+      <c r="A39" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="14.65" thickBot="1">
       <c r="A40" s="5" t="s">
         <v>30</v>
       </c>
@@ -1112,7 +1130,7 @@
         <v>40.292000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="14.65" thickBot="1">
       <c r="A41" s="5" t="s">
         <v>31</v>
       </c>
@@ -1123,7 +1141,7 @@
         <v>40.365000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="14.65" thickBot="1">
       <c r="A42" s="5" t="s">
         <v>32</v>
       </c>
@@ -1134,7 +1152,7 @@
         <v>40.499000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="14.65" thickBot="1">
       <c r="A43" s="5" t="s">
         <v>33</v>
       </c>
@@ -1145,7 +1163,7 @@
         <v>40.1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="14.65" thickBot="1">
       <c r="A44" s="5" t="s">
         <v>34</v>
       </c>
@@ -1156,7 +1174,7 @@
         <v>39.712000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="14.65" thickBot="1">
       <c r="A45" s="5" t="s">
         <v>35</v>
       </c>
@@ -1167,7 +1185,7 @@
         <v>39.520000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="5" t="s">
         <v>36</v>
       </c>
@@ -1178,19 +1196,19 @@
         <v>39.58</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:4" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
+    <row r="48" spans="1:4" ht="18.600000000000001" customHeight="1" thickBot="1">
+      <c r="A48" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+    </row>
+    <row r="49" spans="1:3" ht="14.65" thickBot="1">
       <c r="A49" s="5" t="s">
         <v>37</v>
       </c>
@@ -1201,7 +1219,7 @@
         <v>39.899000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="14.65" thickBot="1">
       <c r="A50" s="5" t="s">
         <v>38</v>
       </c>
@@ -1212,7 +1230,7 @@
         <v>39.875999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="14.65" thickBot="1">
       <c r="A51" s="5" t="s">
         <v>39</v>
       </c>
@@ -1223,7 +1241,7 @@
         <v>39.954000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="14.65" thickBot="1">
       <c r="A52" s="5" t="s">
         <v>40</v>
       </c>
@@ -1234,7 +1252,7 @@
         <v>39.856000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="5" t="s">
         <v>41</v>
       </c>
@@ -1247,6 +1265,9 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A12:C12"/>
     <mergeCell ref="A48:C48"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A26:C26"/>
@@ -1257,11 +1278,533 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="25.46484375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5">
+        <v>116.417</v>
+      </c>
+      <c r="C2" s="5">
+        <v>39.929000000000002</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>116.407</v>
+      </c>
+      <c r="C3" s="5">
+        <v>39.886000000000003</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5">
+        <v>116.339</v>
+      </c>
+      <c r="C4" s="5">
+        <v>39.929000000000002</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
+        <v>116.352</v>
+      </c>
+      <c r="C5" s="5">
+        <v>39.878</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5">
+        <v>116.39700000000001</v>
+      </c>
+      <c r="C6" s="5">
+        <v>39.981999999999999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
+        <v>116.461</v>
+      </c>
+      <c r="C7" s="5">
+        <v>39.936999999999998</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5">
+        <v>116.28700000000001</v>
+      </c>
+      <c r="C8" s="5">
+        <v>39.987000000000002</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5">
+        <v>116.17400000000001</v>
+      </c>
+      <c r="C9" s="5">
+        <v>40.090000000000003</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5">
+        <v>116.20699999999999</v>
+      </c>
+      <c r="C10" s="5">
+        <v>40.002000000000002</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>116.279</v>
+      </c>
+      <c r="C11" s="5">
+        <v>39.863</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5">
+        <v>116.146</v>
+      </c>
+      <c r="C12" s="5">
+        <v>39.823999999999998</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="5">
+        <v>116.184</v>
+      </c>
+      <c r="C13" s="5">
+        <v>39.914000000000001</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="5">
+        <v>116.136</v>
+      </c>
+      <c r="C14" s="5">
+        <v>39.741999999999997</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="5">
+        <v>116.404</v>
+      </c>
+      <c r="C15" s="5">
+        <v>39.718000000000004</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5">
+        <v>116.506</v>
+      </c>
+      <c r="C16" s="5">
+        <v>39.795000000000002</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5">
+        <v>116.663</v>
+      </c>
+      <c r="C17" s="5">
+        <v>39.886000000000003</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5">
+        <v>116.655</v>
+      </c>
+      <c r="C18" s="5">
+        <v>40.127000000000002</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="5">
+        <v>116.23</v>
+      </c>
+      <c r="C19" s="5">
+        <v>40.216999999999999</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5">
+        <v>116.10599999999999</v>
+      </c>
+      <c r="C20" s="5">
+        <v>39.936999999999998</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="5">
+        <v>117.1</v>
+      </c>
+      <c r="C21" s="5">
+        <v>40.143000000000001</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="5">
+        <v>116.628</v>
+      </c>
+      <c r="C22" s="5">
+        <v>40.328000000000003</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="5">
+        <v>116.83199999999999</v>
+      </c>
+      <c r="C23" s="5">
+        <v>40.369999999999997</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="5">
+        <v>115.97199999999999</v>
+      </c>
+      <c r="C24" s="5">
+        <v>40.453000000000003</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="5">
+        <v>116.22</v>
+      </c>
+      <c r="C25" s="5">
+        <v>40.292000000000002</v>
+      </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="5">
+        <v>115.988</v>
+      </c>
+      <c r="C26" s="5">
+        <v>40.365000000000002</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="5">
+        <v>116.911</v>
+      </c>
+      <c r="C27" s="5">
+        <v>40.499000000000002</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="5">
+        <v>117.12</v>
+      </c>
+      <c r="C28" s="5">
+        <v>40.1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="5">
+        <v>116.783</v>
+      </c>
+      <c r="C29" s="5">
+        <v>39.712000000000003</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="5">
+        <v>116.3</v>
+      </c>
+      <c r="C30" s="5">
+        <v>39.520000000000003</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A31" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="5">
+        <v>116</v>
+      </c>
+      <c r="C31" s="5">
+        <v>39.58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="5">
+        <v>116.395</v>
+      </c>
+      <c r="C32" s="5">
+        <v>39.899000000000001</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="5">
+        <v>116.39400000000001</v>
+      </c>
+      <c r="C33" s="5">
+        <v>39.875999999999998</v>
+      </c>
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A34" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="5">
+        <v>116.349</v>
+      </c>
+      <c r="C34" s="5">
+        <v>39.954000000000001</v>
+      </c>
+      <c r="D34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="14.65" thickBot="1">
+      <c r="A35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="5">
+        <v>116.36799999999999</v>
+      </c>
+      <c r="C35" s="5">
+        <v>39.856000000000002</v>
+      </c>
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="5">
+        <v>116.483</v>
+      </c>
+      <c r="C36" s="5">
+        <v>39.939</v>
+      </c>
+      <c r="D36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>